<commit_message>
updating Reg Proc Templates - Added Masked UIN Template
</commit_message>
<xml_diff>
--- a/_files/requirements/master_data/master-template.xlsx
+++ b/_files/requirements/master_data/master-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5EE2B6-6FB6-4061-B1CB-2CB6BC2B8618}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303BF0D4-3B87-4A86-9485-3E5BE589EABB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1184,9 +1184,6 @@
 &lt;/style&gt;&lt;script&gt;function changeColour(element) { var div = document.getElementById("radioId"); if(element.value == "yes"){div.style = "border: 2px solid #68A933";}
 if(element.value == "no"){div.style = "border: 2px solid #FF0000";}}
 document.onreadystatechange = function () {if(document.readyState === "complete"){var body = document.getElementsByTagName("body")[0]; body.addEventListener("dragstart", function(event) {event.preventDefault();}); body.addEventListener("selectstart", function(event) {event.preventDefault();});}}&lt;/script&gt;&lt;/head&gt;</t>
-  </si>
-  <si>
-    <t>MASKED_UIN_CARD_TEMPLATE</t>
   </si>
   <si>
     <t>Masked UIN card template</t>
@@ -2049,6 +2046,9 @@
 	&lt;/table&gt;
 &lt;/body&gt;
 &lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>RPR_MASKED_UIN_CARD_TEMPLATE</t>
   </si>
 </sst>
 </file>
@@ -2898,8 +2898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F180" sqref="F180"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3313,7 +3313,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G11" s="1">
         <v>10003</v>
@@ -3351,7 +3351,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G12" s="1">
         <v>10003</v>
@@ -3389,7 +3389,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G13" s="1">
         <v>10003</v>
@@ -3427,7 +3427,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G14" s="1">
         <v>10003</v>
@@ -3465,7 +3465,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G15" s="1">
         <v>10003</v>
@@ -3503,7 +3503,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G16" s="1">
         <v>10003</v>
@@ -3541,7 +3541,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G17" s="1">
         <v>10003</v>
@@ -3579,7 +3579,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G18" s="1">
         <v>10003</v>
@@ -3617,7 +3617,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G19" s="1">
         <v>10003</v>
@@ -3655,7 +3655,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G20" s="1">
         <v>10003</v>
@@ -3693,7 +3693,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G21" s="1">
         <v>10003</v>
@@ -3731,7 +3731,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G22" s="1">
         <v>10003</v>
@@ -3769,7 +3769,7 @@
         <v>14</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G23" s="1">
         <v>10003</v>
@@ -3807,7 +3807,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G24" s="1">
         <v>10003</v>
@@ -3845,7 +3845,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G25" s="1">
         <v>10003</v>
@@ -3883,7 +3883,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G26" s="1">
         <v>10003</v>
@@ -3921,7 +3921,7 @@
         <v>14</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G27" s="1">
         <v>10003</v>
@@ -3959,7 +3959,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G28" s="1">
         <v>10003</v>
@@ -3997,7 +3997,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G29" s="1">
         <v>10003</v>
@@ -4035,7 +4035,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G30" s="1">
         <v>10003</v>
@@ -4073,7 +4073,7 @@
         <v>14</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G31" s="1">
         <v>10003</v>
@@ -4111,7 +4111,7 @@
         <v>14</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G32" s="1">
         <v>10003</v>
@@ -4149,7 +4149,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G33" s="1">
         <v>10003</v>
@@ -4187,7 +4187,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G34" s="1">
         <v>10003</v>
@@ -6049,7 +6049,7 @@
         <v>198</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G83" s="1">
         <v>10003</v>
@@ -6087,7 +6087,7 @@
         <v>198</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G84" s="1">
         <v>10003</v>
@@ -6125,7 +6125,7 @@
         <v>198</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G85" s="1">
         <v>10003</v>
@@ -6163,7 +6163,7 @@
         <v>14</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G86" s="1">
         <v>10003</v>
@@ -6201,7 +6201,7 @@
         <v>14</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G87" s="1">
         <v>10003</v>
@@ -6239,7 +6239,7 @@
         <v>14</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G88" s="1">
         <v>10003</v>
@@ -6277,7 +6277,7 @@
         <v>14</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G89" s="1">
         <v>10003</v>
@@ -6315,7 +6315,7 @@
         <v>14</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G90" s="1">
         <v>10003</v>
@@ -6353,7 +6353,7 @@
         <v>14</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G91" s="1">
         <v>10003</v>
@@ -6391,7 +6391,7 @@
         <v>14</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G92" s="1">
         <v>10003</v>
@@ -6429,7 +6429,7 @@
         <v>14</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G93" s="1">
         <v>10003</v>
@@ -6467,7 +6467,7 @@
         <v>14</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G94" s="1">
         <v>10003</v>
@@ -6505,7 +6505,7 @@
         <v>14</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G95" s="1">
         <v>10003</v>
@@ -6543,7 +6543,7 @@
         <v>14</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G96" s="1">
         <v>10003</v>
@@ -6581,7 +6581,7 @@
         <v>14</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G97" s="1">
         <v>10003</v>
@@ -7319,7 +7319,7 @@
         <v>252</v>
       </c>
       <c r="F115" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G115">
         <v>10003</v>
@@ -9727,7 +9727,7 @@
         <v>216</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G174" s="1">
         <v>10003</v>
@@ -9768,7 +9768,7 @@
         <v>216</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G175" s="1">
         <v>10003</v>
@@ -9809,7 +9809,7 @@
         <v>216</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G176" s="1">
         <v>10003</v>
@@ -9850,7 +9850,7 @@
         <v>216</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G177" s="1">
         <v>10003</v>
@@ -9891,7 +9891,7 @@
         <v>216</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G178" s="1">
         <v>10003</v>
@@ -9932,7 +9932,7 @@
         <v>216</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G179" s="1">
         <v>10003</v>
@@ -9961,10 +9961,10 @@
         <v>1162</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>14</v>
@@ -9973,7 +9973,7 @@
         <v>216</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G180" s="1">
         <v>10003</v>
@@ -9982,7 +9982,7 @@
         <v>54</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>336</v>
+        <v>383</v>
       </c>
       <c r="J180" s="1" t="s">
         <v>18</v>
@@ -10002,10 +10002,10 @@
         <v>1162</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>14</v>
@@ -10014,7 +10014,7 @@
         <v>216</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G181" s="1">
         <v>10003</v>
@@ -10023,7 +10023,7 @@
         <v>71</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>336</v>
+        <v>383</v>
       </c>
       <c r="J181" s="1" t="s">
         <v>34</v>
@@ -10043,10 +10043,10 @@
         <v>1162</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>14</v>
@@ -10055,7 +10055,7 @@
         <v>216</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G182" s="1">
         <v>10003</v>
@@ -10064,7 +10064,7 @@
         <v>80</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>336</v>
+        <v>383</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
changes in tempate master data
</commit_message>
<xml_diff>
--- a/_files/requirements/master_data/master-template.xlsx
+++ b/_files/requirements/master_data/master-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1681A9-30B1-4E79-BF96-F4E355E9F071}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FE006D-0FD0-4AD2-9785-016982C063CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1191,6 +1191,217 @@
   </si>
   <si>
     <t>RPR_MASKED_UIN_CARD_TEMPLATE</t>
+  </si>
+  <si>
+    <t>$!name_ara ،
+تم إلغاء تنشيط UIN الخاص بك.
+إذا كان لديك أي مواصلات ، يرجى زيارة أقرب مركز للتسجيل.
+شكرا</t>
+  </si>
+  <si>
+    <t>$!name_ara ،
+تمت إعادة تنشيط UIN الخاص بك.
+إذا كان لديك أي مواصلات ، يرجى زيارة أقرب مركز للتسجيل.
+شكرا</t>
+  </si>
+  <si>
+    <t>Dear $name_eng,
+Your UIN for Registration ID: $!RID has been successfully generated and will reach soon at your postal address.
+Thank You</t>
+  </si>
+  <si>
+    <t>Dear $name_eng,
+Your UIN for Registration ID: $!RID has been successfully generated and will reach soon at your postal address.</t>
+  </si>
+  <si>
+    <t>$!name_ara ،
+تم تحديث تفاصيل UIN المطابقة لمعرف التسجيل: $!RID وسوف تصل إليك نسخة مادية من UIN في عنوانك البريدي قريبًا.
+شكرا</t>
+  </si>
+  <si>
+    <t>$!name_ara ،
+تم تحديث تفاصيل UIN المطابقة لمعرف التسجيل: $!RID وسوف تصل إليك نسخة مادية من UIN في عنوانك البريدي قريبًا.</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre UIN a été désactivé.
+Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your UIN has been de-activated. 
+If you have any conserns please visit the nearest Registration Center.</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your UIN has been de-activated. 
+If you have any conserns please visit the nearest Registration Center.
+Thank You</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre UIN a été désactivé.
+Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.
+Merci</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your UIN has been re-activated. 
+If you have any conserns please visit the nearest Registration Center.
+Thank You</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre UIN a été réactivé.
+Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.</t>
+  </si>
+  <si>
+    <t>$!name_ara ،
+تمت إعادة تنشيط UIN الخاص بك.
+إذا كان لديك أي مواصلات ، يرجى زيارة أقرب مركز للتسجيل.</t>
+  </si>
+  <si>
+    <t>Dear $name_eng,
+Your UIN is Found. You will receive your UIN Card soon at your Postal Address.
+Thank You</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre UIN est trouvé. Vous recevrez bientôt votre carte UIN à votre adresse postale.
+Merci</t>
+  </si>
+  <si>
+    <t>$!name_ara،
+تم العثور على UIN الخاص بك. ستتلقى بطاقة UIN الخاصة بك قريبًا على عنوانك البريدي.
+شكرا</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre UIN pour ID d’enregistrement: $!RID a été généré avec succès et vous parviendra sous peu à votre adresse postale.
+Merci</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre UIN pour ID d’enregistrement: $!RID a été généré avec succès et vous parviendra sous peu à votre adresse postale.</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Les détails de votre UIN correspondant à l’ID d’enregistrement: $!RID ont été mis à jour. Une copie physique de votre UIN vous parviendra sous peu à votre adresse postale.
+Merci</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Les détails de votre UIN correspondant à l’ID d’enregistrement: $!RID ont été mis à jour. Une copie physique de votre UIN vous parviendra sous peu à votre adresse postale.</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre UIN a été réactivé.
+Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.
+Merci</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your request for UIN for Registration ID: $!RID has failed because a duplicate UIN has been found against your details. Please visit your nearest Registration office or visit https://mosip.io/grievances
+Thank You</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your request for UIN for Registration ID: $!RID has failed because a duplicate UIN has been found against your details. Please visit your nearest Registration office or visit https://mosip.io/grievances</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your UIN details for the Registration ID: $!RID have been updated and a physical copy of your UIN card will reach you soon at your postal address.
+Thank You</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your UIN details for the Registration ID: $!RID have been updated and a physical copy of your UIN card will reach you soon at your postal address.</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your UIN has been re-activated. 
+If you have any conserns please visit the nearest Registration Center.</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your request for UIN for Registration ID: $!RID has failed because of a technical issue. Please visit your nearest Registration office or visit https://mosip.io/grievances
+Thank You</t>
+  </si>
+  <si>
+    <t>Dear $!name_eng,
+Your request for UIN for Registration ID: $!RID has failed because of a technical issue. Please visit your nearest Registration office or visit https://mosip.io/grievances</t>
+  </si>
+  <si>
+    <t>Dear $name_eng,
+Your UIN is Found. You will receive your UIN Card soon at your Postal Address.</t>
+  </si>
+  <si>
+    <t>$!name_ara،
+لقد فشل طلبك الخاص بـ UIN لمعرف التسجيل: $!RID لأنه تم العثور على UIN مكرر مقابل تفاصيلك. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances
+شكرا جزيلا</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué car un duplicata d'UIN a été trouvé par rapport à vos informations. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances
+Merci</t>
+  </si>
+  <si>
+    <t>$!name_ara،
+لقد فشل طلبك الخاص بـ UIN لمعرف التسجيل: $!RID لأنه تم العثور على UIN مكرر مقابل تفاصيلك. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué car un duplicata d'UIN a été trouvé par rapport à vos informations. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances</t>
+  </si>
+  <si>
+    <t>$!name_ara،
+تم العثور على UIN الخاص بك. ستتلقى بطاقة UIN الخاصة بك قريبًا على عنوانك البريدي.</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué en raison d'un problème technique. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances
+Merci</t>
+  </si>
+  <si>
+    <t>$!name_ara،
+طلبك لـ UIN لمعرف التسجيل: $!RID فشل بسبب مشكلة فنية. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances
+شكرا جزيلا</t>
+  </si>
+  <si>
+    <t>$!name_ara،
+طلبك لـ UIN لمعرف التسجيل: $!RID فشل بسبب مشكلة فنية. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances</t>
+  </si>
+  <si>
+    <t>Cher $!name_fra,
+Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué en raison d'un problème technique. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances</t>
+  </si>
+  <si>
+    <t>$name_ara،
+تم إنشاء رقم UIN الخاص بك لمعرف التسجيل: $!RID بنجاح وسيصل قريباً إلى عنوانك البريدي.
+شكرا جزيلا</t>
+  </si>
+  <si>
+    <t>$name_ara،
+تم إنشاء رقم UIN الخاص بك لمعرف التسجيل: $!RID بنجاح وسيصل قريباً إلى عنوانك البريدي.</t>
+  </si>
+  <si>
+    <t>عزيزي $name ،
+مصادقة UIN $uin باستخدام $authType على $date في $time Hrs $status على جهاز تم نشره بواسطة "خدمات MOSIP".</t>
+  </si>
+  <si>
+    <t>مصادقتك على UIN $uin باستخدام $authType في $date في $time Hrs $status على جهاز تم نشره بواسطة "خدمات MOSIP".</t>
+  </si>
+  <si>
+    <t>Service d'authentification OTP</t>
+  </si>
+  <si>
+    <t>التسجيل</t>
+  </si>
+  <si>
+    <t>Inscription</t>
+  </si>
+  <si>
+    <t>Registration</t>
   </si>
   <si>
     <t>&lt;!DOCTYPE html&gt;
@@ -1254,7 +1465,7 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;Name&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; 
-&lt;span class="name-color"&gt; $!name_eng&lt;/span&gt;
+&lt;span class="name-color"&gt; $!fullName_eng&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1262,15 +1473,15 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;اسم&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; 
-&lt;span&gt;$!name_ara&lt;/span&gt;
+&lt;span&gt;$!fullName_ara&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
 &lt;tr&gt;
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
-&lt;label class="name-head-color"&gt;&lt;b&gt;Date/تاريخ&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt;
-&lt;span&gt;$!dob&lt;/span&gt;
+&lt;label class="name-head-color"&gt;&lt;b&gt;DOB/تاريخ&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt;
+&lt;span&gt;$!dateOfBirth&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1400,7 +1611,7 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;Prénom&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; 
-&lt;span class="name-color"&gt; $!name_eng&lt;/span&gt;
+&lt;span class="name-color"&gt; $!fullName_fra&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1408,7 +1619,7 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;اسم&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; 
-&lt;span&gt;$!name_ara&lt;/span&gt;
+&lt;span&gt;$!fullName_ara&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1416,14 +1627,14 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;Rendez-vous amoureux/تاريخ&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt;
-&lt;span&gt;$!dob&lt;/span&gt;
+&lt;span&gt;$!dateOfBirth&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
 &lt;tr&gt;
 &lt;td colspan="2"&gt;
 &lt;div class="block top-buffer"&gt;
-&lt;label class="name-head-color"&gt;&lt;b&gt;Le sexe&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; &lt;span&gt;$!gender_eng&lt;/span&gt;
+&lt;label class="name-head-color"&gt;&lt;b&gt;Le sexe&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; &lt;span&gt;$!gender_fra&lt;/span&gt;
 &amp;nbsp;&amp;nbsp; &lt;label class="name-head-color"&gt;&lt;b&gt;جنس&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt;
 &lt;span&gt;$!gender_ara&lt;/span&gt;
 &lt;/div&gt;
@@ -1438,8 +1649,8 @@
 &lt;tr&gt;
 &lt;td&gt;&lt;label class="name-head-color"&gt;&lt;b&gt;Adresse&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt;
 &lt;/td&gt;
-&lt;td&gt;&lt;span&gt;$!addressLine1_eng, $!addressLine2_eng,
-		$!addressLine3_eng, $!region_eng, $!province_eng, $!city_eng,
+&lt;td&gt;&lt;span&gt;$!addressLine1_fra, $!addressLine2_fra,
+		$!addressLine3_fra, $!region_fra, $!province_fra, $!city_fra,
 		$!postalCode &lt;/span&gt;&lt;/td&gt;
 &lt;/tr&gt;
 &lt;tr&gt;
@@ -1483,6 +1694,10 @@
 &lt;/table&gt;
 &lt;/body&gt;
 &lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>Cher $!name_fr+F180a,
+Votre UIN est trouvé. Vous recevrez bientôt votre carte UIN à votre adresse postale.</t>
   </si>
   <si>
     <t>&lt;!DOCTYPE html&gt;
@@ -1554,14 +1769,14 @@
 &lt;tr&gt;
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
-&lt;label class="name-head-color"&gt;&lt;b&gt;Name&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; &lt;span class="name-color"&gt; $!name_eng&lt;/span&gt;
+&lt;label class="name-head-color"&gt;&lt;b&gt;Name&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; &lt;span class="name-color"&gt; $!fullName_eng&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
 &lt;tr&gt;
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
-&lt;label class="name-head-color"&gt;&lt;b&gt;اسم&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; &lt;span&gt; $!name_ara&lt;/span&gt;
+&lt;label class="name-head-color"&gt;&lt;b&gt;اسم&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; &lt;span&gt; $!fullName_ara&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1704,7 +1919,7 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;Prénom&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; 
-&lt;span class="name-color"&gt; $!name_eng&lt;/span&gt;
+&lt;span class="name-color"&gt; $!fullName_fra&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1712,7 +1927,7 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;اسم&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt; 
-&lt;span&gt;$!name_ara&lt;/span&gt;
+&lt;span&gt;$!fullName_ara&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1720,7 +1935,7 @@
 &lt;td rowspan="1"&gt;
 &lt;div class="block top-buffer"&gt;
 &lt;label class="name-head-color"&gt;&lt;b&gt;Rendez-vous amoureux/تاريخ&amp;nbsp;:&amp;nbsp;&lt;/b&gt;&lt;/label&gt;
-&lt;span&gt;$!dob&lt;/span&gt;
+&lt;span&gt;$!dateOfBirth&lt;/span&gt;
 &lt;/div&gt;
 &lt;/td&gt;
 &lt;/tr&gt;
@@ -1787,221 +2002,6 @@
 &lt;/table&gt;
 &lt;/body&gt;
 &lt;/html&gt;</t>
-  </si>
-  <si>
-    <t>$!name_ara ،
-تم إلغاء تنشيط UIN الخاص بك.
-إذا كان لديك أي مواصلات ، يرجى زيارة أقرب مركز للتسجيل.
-شكرا</t>
-  </si>
-  <si>
-    <t>$!name_ara ،
-تمت إعادة تنشيط UIN الخاص بك.
-إذا كان لديك أي مواصلات ، يرجى زيارة أقرب مركز للتسجيل.
-شكرا</t>
-  </si>
-  <si>
-    <t>Dear $name_eng,
-Your UIN for Registration ID: $!RID has been successfully generated and will reach soon at your postal address.
-Thank You</t>
-  </si>
-  <si>
-    <t>Dear $name_eng,
-Your UIN for Registration ID: $!RID has been successfully generated and will reach soon at your postal address.</t>
-  </si>
-  <si>
-    <t>$!name_ara ،
-تم تحديث تفاصيل UIN المطابقة لمعرف التسجيل: $!RID وسوف تصل إليك نسخة مادية من UIN في عنوانك البريدي قريبًا.
-شكرا</t>
-  </si>
-  <si>
-    <t>$!name_ara ،
-تم تحديث تفاصيل UIN المطابقة لمعرف التسجيل: $!RID وسوف تصل إليك نسخة مادية من UIN في عنوانك البريدي قريبًا.</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN a été désactivé.
-Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your UIN has been de-activated. 
-If you have any conserns please visit the nearest Registration Center.</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your UIN has been de-activated. 
-If you have any conserns please visit the nearest Registration Center.
-Thank You</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN a été désactivé.
-Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.
-Merci</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your UIN has been re-activated. 
-If you have any conserns please visit the nearest Registration Center.
-Thank You</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN a été réactivé.
-Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.</t>
-  </si>
-  <si>
-    <t>$!name_ara ،
-تمت إعادة تنشيط UIN الخاص بك.
-إذا كان لديك أي مواصلات ، يرجى زيارة أقرب مركز للتسجيل.</t>
-  </si>
-  <si>
-    <t>Dear $name_eng,
-Your UIN is Found. You will receive your UIN Card soon at your Postal Address.
-Thank You</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN est trouvé. Vous recevrez bientôt votre carte UIN à votre adresse postale.
-Merci</t>
-  </si>
-  <si>
-    <t>$!name_ara،
-تم العثور على UIN الخاص بك. ستتلقى بطاقة UIN الخاصة بك قريبًا على عنوانك البريدي.
-شكرا</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN pour ID d’enregistrement: $!RID a été généré avec succès et vous parviendra sous peu à votre adresse postale.
-Merci</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN pour ID d’enregistrement: $!RID a été généré avec succès et vous parviendra sous peu à votre adresse postale.</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Les détails de votre UIN correspondant à l’ID d’enregistrement: $!RID ont été mis à jour. Une copie physique de votre UIN vous parviendra sous peu à votre adresse postale.
-Merci</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Les détails de votre UIN correspondant à l’ID d’enregistrement: $!RID ont été mis à jour. Une copie physique de votre UIN vous parviendra sous peu à votre adresse postale.</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN a été réactivé.
-Si vous avez des intérêts, veuillez vous rendre au centre d’enregistrement le plus proche.
-Merci</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your request for UIN for Registration ID: $!RID has failed because a duplicate UIN has been found against your details. Please visit your nearest Registration office or visit https://mosip.io/grievances
-Thank You</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your request for UIN for Registration ID: $!RID has failed because a duplicate UIN has been found against your details. Please visit your nearest Registration office or visit https://mosip.io/grievances</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your UIN details for the Registration ID: $!RID have been updated and a physical copy of your UIN card will reach you soon at your postal address.
-Thank You</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your UIN details for the Registration ID: $!RID have been updated and a physical copy of your UIN card will reach you soon at your postal address.</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your UIN has been re-activated. 
-If you have any conserns please visit the nearest Registration Center.</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your request for UIN for Registration ID: $!RID has failed because of a technical issue. Please visit your nearest Registration office or visit https://mosip.io/grievances
-Thank You</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng,
-Your request for UIN for Registration ID: $!RID has failed because of a technical issue. Please visit your nearest Registration office or visit https://mosip.io/grievances</t>
-  </si>
-  <si>
-    <t>Dear $name_eng,
-Your UIN is Found. You will receive your UIN Card soon at your Postal Address.</t>
-  </si>
-  <si>
-    <t>$!name_ara،
-لقد فشل طلبك الخاص بـ UIN لمعرف التسجيل: $!RID لأنه تم العثور على UIN مكرر مقابل تفاصيلك. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances
-شكرا جزيلا</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué car un duplicata d'UIN a été trouvé par rapport à vos informations. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances
-Merci</t>
-  </si>
-  <si>
-    <t>$!name_ara،
-لقد فشل طلبك الخاص بـ UIN لمعرف التسجيل: $!RID لأنه تم العثور على UIN مكرر مقابل تفاصيلك. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué car un duplicata d'UIN a été trouvé par rapport à vos informations. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre UIN est trouvé. Vous recevrez bientôt votre carte UIN à votre adresse postale.</t>
-  </si>
-  <si>
-    <t>$!name_ara،
-تم العثور على UIN الخاص بك. ستتلقى بطاقة UIN الخاصة بك قريبًا على عنوانك البريدي.</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué en raison d'un problème technique. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances
-Merci</t>
-  </si>
-  <si>
-    <t>$!name_ara،
-طلبك لـ UIN لمعرف التسجيل: $!RID فشل بسبب مشكلة فنية. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances
-شكرا جزيلا</t>
-  </si>
-  <si>
-    <t>$!name_ara،
-طلبك لـ UIN لمعرف التسجيل: $!RID فشل بسبب مشكلة فنية. يرجى زيارة أقرب مكتب للتسجيل أو زيارة https://mosip.io/grievances</t>
-  </si>
-  <si>
-    <t>Cher $!name_fra,
-Votre demande d'UIN pour l'ID d'enregistrement: $!RID a échoué en raison d'un problème technique. Veuillez vous rendre au bureau d’enregistrement le plus proche ou sur https://mosip.io/grievances</t>
-  </si>
-  <si>
-    <t>$name_ara،
-تم إنشاء رقم UIN الخاص بك لمعرف التسجيل: $!RID بنجاح وسيصل قريباً إلى عنوانك البريدي.
-شكرا جزيلا</t>
-  </si>
-  <si>
-    <t>$name_ara،
-تم إنشاء رقم UIN الخاص بك لمعرف التسجيل: $!RID بنجاح وسيصل قريباً إلى عنوانك البريدي.</t>
-  </si>
-  <si>
-    <t>عزيزي $name ،
-مصادقة UIN $uin باستخدام $authType على $date في $time Hrs $status على جهاز تم نشره بواسطة "خدمات MOSIP".</t>
-  </si>
-  <si>
-    <t>مصادقتك على UIN $uin باستخدام $authType في $date في $time Hrs $status على جهاز تم نشره بواسطة "خدمات MOSIP".</t>
-  </si>
-  <si>
-    <t>Service d'authentification OTP</t>
-  </si>
-  <si>
-    <t>التسجيل</t>
-  </si>
-  <si>
-    <t>Inscription</t>
-  </si>
-  <si>
-    <t>Registration</t>
   </si>
 </sst>
 </file>
@@ -2852,7 +2852,7 @@
   <dimension ref="A1:M182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3038,7 +3038,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G5" s="1">
         <v>10004</v>
@@ -3114,7 +3114,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G7" s="1">
         <v>10004</v>
@@ -3266,7 +3266,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G11" s="1">
         <v>10003</v>
@@ -3304,7 +3304,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="G12" s="1">
         <v>10003</v>
@@ -3342,7 +3342,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="G13" s="1">
         <v>10003</v>
@@ -3380,7 +3380,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="G14" s="1">
         <v>10003</v>
@@ -3418,7 +3418,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G15" s="1">
         <v>10003</v>
@@ -3456,7 +3456,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G16" s="1">
         <v>10003</v>
@@ -3494,7 +3494,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G17" s="1">
         <v>10003</v>
@@ -3532,7 +3532,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G18" s="1">
         <v>10003</v>
@@ -3570,7 +3570,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G19" s="1">
         <v>10003</v>
@@ -3608,7 +3608,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G20" s="1">
         <v>10003</v>
@@ -3646,7 +3646,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G21" s="1">
         <v>10003</v>
@@ -3684,7 +3684,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="G22" s="1">
         <v>10003</v>
@@ -3722,7 +3722,7 @@
         <v>14</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G23" s="1">
         <v>10003</v>
@@ -3760,7 +3760,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="G24" s="1">
         <v>10003</v>
@@ -3798,7 +3798,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G25" s="1">
         <v>10003</v>
@@ -3836,7 +3836,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G26" s="1">
         <v>10003</v>
@@ -3874,7 +3874,7 @@
         <v>14</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G27" s="1">
         <v>10003</v>
@@ -3912,7 +3912,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G28" s="1">
         <v>10003</v>
@@ -3950,7 +3950,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="G29" s="1">
         <v>10003</v>
@@ -3988,7 +3988,7 @@
         <v>14</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="G30" s="1">
         <v>10003</v>
@@ -4026,7 +4026,7 @@
         <v>14</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G31" s="1">
         <v>10003</v>
@@ -4064,7 +4064,7 @@
         <v>14</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G32" s="1">
         <v>10003</v>
@@ -4102,7 +4102,7 @@
         <v>14</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G33" s="1">
         <v>10003</v>
@@ -4140,7 +4140,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G34" s="1">
         <v>10003</v>
@@ -6002,7 +6002,7 @@
         <v>198</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>338</v>
+        <v>384</v>
       </c>
       <c r="G83" s="1">
         <v>10003</v>
@@ -6040,7 +6040,7 @@
         <v>198</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>339</v>
+        <v>385</v>
       </c>
       <c r="G84" s="1">
         <v>10003</v>
@@ -6078,7 +6078,7 @@
         <v>198</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>339</v>
+        <v>385</v>
       </c>
       <c r="G85" s="1">
         <v>10003</v>
@@ -6116,7 +6116,7 @@
         <v>14</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G86" s="1">
         <v>10003</v>
@@ -6192,7 +6192,7 @@
         <v>14</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G88" s="1">
         <v>10003</v>
@@ -6230,7 +6230,7 @@
         <v>14</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="G89" s="1">
         <v>10003</v>
@@ -6268,7 +6268,7 @@
         <v>14</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="G90" s="1">
         <v>10003</v>
@@ -6306,7 +6306,7 @@
         <v>14</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G91" s="1">
         <v>10003</v>
@@ -6344,7 +6344,7 @@
         <v>14</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G92" s="1">
         <v>10003</v>
@@ -6382,7 +6382,7 @@
         <v>14</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G93" s="1">
         <v>10003</v>
@@ -6420,7 +6420,7 @@
         <v>14</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G94" s="1">
         <v>10003</v>
@@ -6458,7 +6458,7 @@
         <v>14</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G95" s="1">
         <v>10003</v>
@@ -6496,7 +6496,7 @@
         <v>14</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G96" s="1">
         <v>10003</v>
@@ -6534,7 +6534,7 @@
         <v>14</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G97" s="1">
         <v>10003</v>
@@ -6581,7 +6581,7 @@
         <v>10005</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>217</v>
@@ -6622,7 +6622,7 @@
         <v>10005</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>217</v>
@@ -6663,7 +6663,7 @@
         <v>10005</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>217</v>
@@ -6704,7 +6704,7 @@
         <v>10005</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>223</v>
@@ -6745,7 +6745,7 @@
         <v>10005</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>223</v>
@@ -6786,7 +6786,7 @@
         <v>10005</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>223</v>
@@ -6827,7 +6827,7 @@
         <v>10005</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>229</v>
@@ -6868,7 +6868,7 @@
         <v>10005</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>229</v>
@@ -6909,7 +6909,7 @@
         <v>10005</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>229</v>
@@ -6950,7 +6950,7 @@
         <v>10005</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>230</v>
@@ -6991,7 +6991,7 @@
         <v>10005</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>230</v>
@@ -7032,7 +7032,7 @@
         <v>10005</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>230</v>
@@ -7073,7 +7073,7 @@
         <v>10005</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>231</v>
@@ -7114,7 +7114,7 @@
         <v>10005</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>231</v>
@@ -7155,7 +7155,7 @@
         <v>10005</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>231</v>
@@ -7360,7 +7360,7 @@
         <v>10005</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>263</v>
@@ -7401,7 +7401,7 @@
         <v>10005</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>263</v>
@@ -7442,7 +7442,7 @@
         <v>10005</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>263</v>
@@ -7875,7 +7875,7 @@
         <v>1145</v>
       </c>
       <c r="B130" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C130" t="s">
         <v>279</v>
@@ -9071,7 +9071,7 @@
         <v>10005</v>
       </c>
       <c r="H159" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I159" t="s">
         <v>298</v>
@@ -9112,7 +9112,7 @@
         <v>10005</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I160" t="s">
         <v>298</v>
@@ -9153,7 +9153,7 @@
         <v>10005</v>
       </c>
       <c r="H161" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I161" t="s">
         <v>298</v>
@@ -9194,7 +9194,7 @@
         <v>10005</v>
       </c>
       <c r="H162" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I162" t="s">
         <v>304</v>
@@ -9235,7 +9235,7 @@
         <v>10005</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I163" t="s">
         <v>304</v>
@@ -9276,7 +9276,7 @@
         <v>10005</v>
       </c>
       <c r="H164" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I164" t="s">
         <v>304</v>
@@ -9317,7 +9317,7 @@
         <v>10005</v>
       </c>
       <c r="H165" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I165" t="s">
         <v>307</v>
@@ -9358,7 +9358,7 @@
         <v>10005</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I166" t="s">
         <v>307</v>
@@ -9399,7 +9399,7 @@
         <v>10005</v>
       </c>
       <c r="H167" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I167" t="s">
         <v>307</v>
@@ -9440,7 +9440,7 @@
         <v>10005</v>
       </c>
       <c r="H168" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="I168" t="s">
         <v>310</v>
@@ -9481,7 +9481,7 @@
         <v>10005</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I169" t="s">
         <v>310</v>
@@ -9522,7 +9522,7 @@
         <v>10005</v>
       </c>
       <c r="H170" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I170" t="s">
         <v>310</v>
@@ -9680,7 +9680,7 @@
         <v>216</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G174" s="1">
         <v>10003</v>
@@ -9721,7 +9721,7 @@
         <v>216</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G175" s="1">
         <v>10003</v>
@@ -9762,7 +9762,7 @@
         <v>216</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="G176" s="1">
         <v>10003</v>
@@ -9803,7 +9803,7 @@
         <v>216</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G177" s="1">
         <v>10003</v>
@@ -9844,7 +9844,7 @@
         <v>216</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G178" s="1">
         <v>10003</v>
@@ -9885,7 +9885,7 @@
         <v>216</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G179" s="1">
         <v>10003</v>
@@ -9926,7 +9926,7 @@
         <v>216</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>340</v>
+        <v>387</v>
       </c>
       <c r="G180" s="1">
         <v>10003</v>
@@ -9967,7 +9967,7 @@
         <v>216</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>341</v>
+        <v>388</v>
       </c>
       <c r="G181" s="1">
         <v>10003</v>
@@ -10008,7 +10008,7 @@
         <v>216</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>341</v>
+        <v>388</v>
       </c>
       <c r="G182" s="1">
         <v>10003</v>

</xml_diff>